<commit_message>
- Fix some email template issue
</commit_message>
<xml_diff>
--- a/Server/src/DemoFiles/add_subject.xlsx
+++ b/Server/src/DemoFiles/add_subject.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhruv\Downloads\ERP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Web_Development_Projects\ERP\Server\src\DemoFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{329F0B1C-6F42-4D02-9505-4B7F1DA19C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97BAAB1-4ED1-4479-8174-342E9B65F9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{44E21A46-72CB-4194-AF0D-B9649DD95D77}"/>
   </bookViews>
@@ -27,16 +27,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>sem</t>
   </si>
   <si>
     <t>branchId</t>
+  </si>
+  <si>
+    <t>subject_code</t>
+  </si>
+  <si>
+    <t>subject_name</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,16 +404,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>